<commit_message>
Implemented more formula features
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkri\IdeaProjects\eba-rules-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA23ACA-5A88-4495-B276-C750AC2B3313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EC8EF-F75E-4485-AD11-6559AE522472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="Eins" sheetId="1" r:id="rId1"/>
+    <sheet name="Zwei" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Row</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>Bla</t>
+  </si>
+  <si>
+    <t>Katze</t>
   </si>
 </sst>
 </file>
@@ -429,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F4"/>
+  <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +446,7 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -458,8 +462,11 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -477,8 +484,12 @@
         <f>"0040"</f>
         <v>0040</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="str">
+        <f>"0080"</f>
+        <v>0080</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>"0100"</f>
         <v>0100</v>
@@ -496,8 +507,11 @@
       <c r="F3">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>"0200"</f>
         <v>0200</v>
@@ -514,6 +528,421 @@
       </c>
       <c r="F4">
         <v>26</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="str">
+        <f>"0300"</f>
+        <v>0300</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" ref="C5:C11" si="0">"1.2"</f>
+        <v>1.2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>67</v>
+      </c>
+      <c r="F5">
+        <v>412</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="str">
+        <f>"0400"</f>
+        <v>0400</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="str">
+        <f>"0500"</f>
+        <v>0500</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="str">
+        <f>"0600"</f>
+        <v>0600</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="str">
+        <f>"0700"</f>
+        <v>0700</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>66</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="str">
+        <f>"0800"</f>
+        <v>0800</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>345</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="str">
+        <f>"0900"</f>
+        <v>0900</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E06B16-6E18-457F-810E-325A834D49B1}">
+  <dimension ref="B1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>"0030"</f>
+        <v>0030</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>"0040"</f>
+        <v>0040</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>"0080"</f>
+        <v>0080</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="str">
+        <f>"0100"</f>
+        <v>0100</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>"1.1"</f>
+        <v>1.1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1337</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="str">
+        <f>"0200"</f>
+        <v>0200</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>"1.2"</f>
+        <v>1.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="str">
+        <f>"0300"</f>
+        <v>0300</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" ref="C5:C11" si="0">"1.2"</f>
+        <v>1.2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>67</v>
+      </c>
+      <c r="F5">
+        <v>412</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="str">
+        <f>"0400"</f>
+        <v>0400</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="str">
+        <f>"0500"</f>
+        <v>0500</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="str">
+        <f>"0600"</f>
+        <v>0600</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="str">
+        <f>"0700"</f>
+        <v>0700</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>66</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="str">
+        <f>"0800"</f>
+        <v>0800</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>345</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="str">
+        <f>"0900"</f>
+        <v>0900</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented row / column permutation support
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkri\IdeaProjects\eba-rules-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EC8EF-F75E-4485-AD11-6559AE522472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9761657A-1614-4657-BF44-862FC7C4A24A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="9705" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eins" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>1</v>

</xml_diff>

<commit_message>
Added support for sum({(rNNN)})
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkri\IdeaProjects\eba-rules-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9761657A-1614-4657-BF44-862FC7C4A24A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8621E300-3763-4D9C-A15B-6F9EE88FEB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="9705" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-225" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eins" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>